<commit_message>
Last small fixes for v1.11
</commit_message>
<xml_diff>
--- a/rp2350b-launchpad-PCB-BOM.xlsx
+++ b/rp2350b-launchpad-PCB-BOM.xlsx
@@ -115,7 +115,7 @@
     <t xml:space="preserve">LED_SMD:LED_0603_1608Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">C2290</t>
+    <t xml:space="preserve">C84269</t>
   </si>
   <si>
     <t xml:space="preserve">PWR</t>
@@ -561,10 +561,10 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D43"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.36"/>

</xml_diff>